<commit_message>
Update Báo cáo tài chính
Sửa báo cáo tài chính
- Nhật ký thu tiền
- Nhật ký chi tiền
- Sổ quỹ
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Report/BaoCaoTaiChinh/Teamplate_BaoCaoNhatKyChiTien.xlsx
+++ b/banhang24/Template/ExportExcel/Report/BaoCaoTaiChinh/Teamplate_BaoCaoNhatKyChiTien.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80071AC-B188-4EB9-8458-AF4E41814649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,12 +13,24 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$4:$4</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Tổng cộng:</t>
   </si>
@@ -43,9 +56,6 @@
     <t>Tên người nhận</t>
   </si>
   <si>
-    <t>Tổng tiền chi</t>
-  </si>
-  <si>
     <t>Khoản mục</t>
   </si>
   <si>
@@ -56,12 +66,27 @@
   </si>
   <si>
     <t>Chi nhánh</t>
+  </si>
+  <si>
+    <t>Tiền mặt</t>
+  </si>
+  <si>
+    <t>Chuyển khoản</t>
+  </si>
+  <si>
+    <t>Visa</t>
+  </si>
+  <si>
+    <t>Số tài khoản</t>
+  </si>
+  <si>
+    <t>Ngân hàng</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
@@ -385,6 +410,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -420,6 +462,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -595,12 +654,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:K1"/>
+      <selection pane="bottomLeft" sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,14 +669,14 @@
     <col min="4" max="4" width="16.42578125" style="25" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" style="24" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="7" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" style="21" customWidth="1"/>
-    <col min="9" max="10" width="14.7109375" style="18" customWidth="1"/>
-    <col min="11" max="11" width="29.85546875" style="14" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="9" width="14.7109375" style="7" customWidth="1"/>
+    <col min="10" max="12" width="16.42578125" style="21" customWidth="1"/>
+    <col min="13" max="14" width="14.7109375" style="18" customWidth="1"/>
+    <col min="15" max="15" width="29.85546875" style="14" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>1</v>
       </c>
@@ -631,9 +690,13 @@
       <c r="I1" s="29"/>
       <c r="J1" s="29"/>
       <c r="K1" s="29"/>
-      <c r="L1" s="2"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="30"/>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
@@ -645,12 +708,16 @@
       <c r="I2" s="30"/>
       <c r="J2" s="30"/>
       <c r="K2" s="30"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
     </row>
-    <row r="4" spans="1:12" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
@@ -670,22 +737,34 @@
         <v>7</v>
       </c>
       <c r="G4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="M4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="N4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="O4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -693,12 +772,16 @@
       <c r="E5" s="22"/>
       <c r="F5" s="3"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
       <c r="J5" s="19"/>
-      <c r="K5" s="16"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="16"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -706,12 +789,16 @@
       <c r="E6" s="22"/>
       <c r="F6" s="3"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
       <c r="J6" s="19"/>
-      <c r="K6" s="16"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="16"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -719,12 +806,16 @@
       <c r="E7" s="22"/>
       <c r="F7" s="3"/>
       <c r="G7" s="6"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
       <c r="J7" s="19"/>
-      <c r="K7" s="16"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="16"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -732,12 +823,16 @@
       <c r="E8" s="22"/>
       <c r="F8" s="3"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
       <c r="J8" s="19"/>
-      <c r="K8" s="16"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="16"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -745,12 +840,16 @@
       <c r="E9" s="22"/>
       <c r="F9" s="3"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
       <c r="J9" s="19"/>
-      <c r="K9" s="16"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="16"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -758,12 +857,16 @@
       <c r="E10" s="22"/>
       <c r="F10" s="3"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
       <c r="J10" s="19"/>
-      <c r="K10" s="16"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="16"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -771,12 +874,16 @@
       <c r="E11" s="22"/>
       <c r="F11" s="3"/>
       <c r="G11" s="6"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
       <c r="J11" s="19"/>
-      <c r="K11" s="16"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="16"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -784,12 +891,16 @@
       <c r="E12" s="22"/>
       <c r="F12" s="3"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
       <c r="J12" s="19"/>
-      <c r="K12" s="16"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="16"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -797,12 +908,16 @@
       <c r="E13" s="22"/>
       <c r="F13" s="3"/>
       <c r="G13" s="6"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
       <c r="J13" s="19"/>
-      <c r="K13" s="16"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="16"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -810,12 +925,16 @@
       <c r="E14" s="22"/>
       <c r="F14" s="3"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
       <c r="J14" s="19"/>
-      <c r="K14" s="16"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="16"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -823,12 +942,16 @@
       <c r="E15" s="22"/>
       <c r="F15" s="3"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
       <c r="J15" s="19"/>
-      <c r="K15" s="16"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="16"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -836,12 +959,16 @@
       <c r="E16" s="22"/>
       <c r="F16" s="3"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
       <c r="J16" s="19"/>
-      <c r="K16" s="16"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="16"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -849,12 +976,16 @@
       <c r="E17" s="22"/>
       <c r="F17" s="3"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
       <c r="J17" s="19"/>
-      <c r="K17" s="16"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="16"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -862,12 +993,16 @@
       <c r="E18" s="22"/>
       <c r="F18" s="3"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
       <c r="J18" s="19"/>
-      <c r="K18" s="16"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="16"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -875,12 +1010,16 @@
       <c r="E19" s="22"/>
       <c r="F19" s="3"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
       <c r="J19" s="19"/>
-      <c r="K19" s="16"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="16"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -888,12 +1027,16 @@
       <c r="E20" s="22"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
       <c r="J20" s="19"/>
-      <c r="K20" s="16"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="16"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -901,12 +1044,16 @@
       <c r="E21" s="22"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
       <c r="J21" s="19"/>
-      <c r="K21" s="16"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="16"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -914,12 +1061,16 @@
       <c r="E22" s="22"/>
       <c r="F22" s="3"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
       <c r="J22" s="19"/>
-      <c r="K22" s="16"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="16"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -927,12 +1078,16 @@
       <c r="E23" s="22"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
       <c r="J23" s="19"/>
-      <c r="K23" s="16"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="16"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -940,12 +1095,16 @@
       <c r="E24" s="22"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
       <c r="J24" s="19"/>
-      <c r="K24" s="16"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="16"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -953,12 +1112,16 @@
       <c r="E25" s="22"/>
       <c r="F25" s="3"/>
       <c r="G25" s="6"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
       <c r="J25" s="19"/>
-      <c r="K25" s="16"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="16"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -966,12 +1129,16 @@
       <c r="E26" s="22"/>
       <c r="F26" s="3"/>
       <c r="G26" s="6"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
       <c r="J26" s="19"/>
-      <c r="K26" s="16"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="16"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -979,12 +1146,16 @@
       <c r="E27" s="22"/>
       <c r="F27" s="3"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
       <c r="J27" s="19"/>
-      <c r="K27" s="16"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="16"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -992,12 +1163,16 @@
       <c r="E28" s="22"/>
       <c r="F28" s="3"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
       <c r="J28" s="19"/>
-      <c r="K28" s="16"/>
-    </row>
-    <row r="29" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="16"/>
+    </row>
+    <row r="29" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
         <v>0</v>
       </c>
@@ -1010,15 +1185,25 @@
         <f>SUM(G$5:G28)</f>
         <v>0</v>
       </c>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
+      <c r="H29" s="8">
+        <f>SUM(H$5:H28)</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="8">
+        <f>SUM(I$5:I28)</f>
+        <v>0</v>
+      </c>
       <c r="J29" s="20"/>
-      <c r="K29" s="17"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:O2"/>
     <mergeCell ref="A29:C29"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>

</xml_diff>